<commit_message>
era diez elevado a 1
</commit_message>
<xml_diff>
--- a/datos_presion_U2.xlsx
+++ b/datos_presion_U2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javier/Documents/University/5th_semester/Experimental_physics/Unidad2_Vacio/Unidad/datos/manejo_datos_presion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F17D74-851A-0142-B197-7F80E15BA2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0547F3BA-52D5-DE41-846A-18208889226F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44840" yWindow="-5600" windowWidth="19160" windowHeight="21600" xr2:uid="{3053025F-C178-CE47-9F28-E3AF749DE76E}"/>
+    <workbookView xWindow="36520" yWindow="-5160" windowWidth="19160" windowHeight="21160" xr2:uid="{3053025F-C178-CE47-9F28-E3AF749DE76E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,7 +424,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>38</v>

</xml_diff>

<commit_message>
Se añade un plot
</commit_message>
<xml_diff>
--- a/datos_presion_U2.xlsx
+++ b/datos_presion_U2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javier/Documents/University/5th_semester/Experimental_physics/Unidad2_Vacio/Unidad/datos/manejo_datos_presion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0547F3BA-52D5-DE41-846A-18208889226F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A34908-364C-114E-BA82-7341B3D982B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36520" yWindow="-5160" windowWidth="19160" windowHeight="21160" xr2:uid="{3053025F-C178-CE47-9F28-E3AF749DE76E}"/>
+    <workbookView xWindow="35480" yWindow="-5160" windowWidth="19160" windowHeight="21160" xr2:uid="{3053025F-C178-CE47-9F28-E3AF749DE76E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>presion_rotatoria(mbar)</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>tiempo_difusora(min)</t>
+  </si>
+  <si>
+    <t>tiempo_d-r</t>
+  </si>
+  <si>
+    <t>presion_d-r(mTorr)</t>
   </si>
 </sst>
 </file>
@@ -397,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9496276-1D6F-2C4D-9917-5BAF9DDAF689}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -418,8 +424,14 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
@@ -433,8 +445,14 @@
         <f>8.1*100</f>
         <v>810</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>58</v>
+      </c>
+      <c r="F2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -448,8 +466,14 @@
         <f>1.6*10</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>47</v>
       </c>
@@ -463,8 +487,14 @@
         <f>7.4*0.1</f>
         <v>0.7400000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>60</v>
       </c>
@@ -478,8 +508,14 @@
         <f>2.6*0.1</f>
         <v>0.26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>47</v>
       </c>
@@ -487,8 +523,14 @@
         <f>2.3*0.1</f>
         <v>0.22999999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>75</v>
+      </c>
+      <c r="F6">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>50</v>
       </c>
@@ -496,8 +538,14 @@
         <f>2.1*0.1</f>
         <v>0.21000000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>80</v>
+      </c>
+      <c r="F7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>55</v>
       </c>
@@ -505,8 +553,14 @@
         <f>2*0.1</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>85</v>
+      </c>
+      <c r="F8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>60</v>
       </c>
@@ -514,8 +568,14 @@
         <f>2*0.1</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>90</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>65</v>
       </c>
@@ -523,8 +583,14 @@
         <f>1.9*0.1</f>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>95</v>
+      </c>
+      <c r="F10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>70</v>
       </c>
@@ -532,8 +598,14 @@
         <f>1.9*0.1</f>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>76</v>
       </c>
@@ -541,8 +613,14 @@
         <f>1.8*0.1</f>
         <v>0.18000000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>105</v>
+      </c>
+      <c r="F12">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>81</v>
       </c>
@@ -550,8 +628,14 @@
         <f>1.8*0.1</f>
         <v>0.18000000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>110</v>
+      </c>
+      <c r="F13">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>85</v>
       </c>
@@ -559,14 +643,34 @@
         <f>1.8*0.1</f>
         <v>0.18000000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>120</v>
+      </c>
+      <c r="F14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>92</v>
       </c>
       <c r="D15">
         <f>1.7*0.1</f>
         <v>0.17</v>
+      </c>
+      <c r="E15">
+        <v>135</v>
+      </c>
+      <c r="F15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>153</v>
+      </c>
+      <c r="F16">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>